<commit_message>
Lire un fichier excel
</commit_message>
<xml_diff>
--- a/Output/Annuaire.xlsx
+++ b/Output/Annuaire.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Worksheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>LOGIN</t>
   </si>
@@ -27,45 +27,48 @@
     <t>NOM</t>
   </si>
   <si>
+    <t>PRENOM</t>
+  </si>
+  <si>
+    <t>TELEPHONE</t>
+  </si>
+  <si>
+    <t>NUM_RUE</t>
+  </si>
+  <si>
+    <t>NOM_RUE</t>
+  </si>
+  <si>
+    <t>CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>VILLE</t>
+  </si>
+  <si>
+    <t>PAYS</t>
+  </si>
+  <si>
+    <t>vasi</t>
+  </si>
+  <si>
+    <t>vasjana</t>
+  </si>
+  <si>
+    <t>spaho</t>
+  </si>
+  <si>
+    <t>place arnold</t>
+  </si>
+  <si>
+    <t>strasbourg</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
     <t>bukuroshi</t>
   </si>
   <si>
-    <t>TELEPHONE</t>
-  </si>
-  <si>
-    <t>NUM_RUE</t>
-  </si>
-  <si>
-    <t>NOM_RUE</t>
-  </si>
-  <si>
-    <t>CODE_POSTAL</t>
-  </si>
-  <si>
-    <t>VILLE</t>
-  </si>
-  <si>
-    <t>PAYS</t>
-  </si>
-  <si>
-    <t>vasi</t>
-  </si>
-  <si>
-    <t>vasjana</t>
-  </si>
-  <si>
-    <t>spaho</t>
-  </si>
-  <si>
-    <t>place arnold</t>
-  </si>
-  <si>
-    <t>strasbourg</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
     <t>bahi</t>
   </si>
   <si>
@@ -136,12 +139,31 @@
   </si>
   <si>
     <t>varret e francezeve</t>
+  </si>
+  <si>
+    <t>mig</t>
+  </si>
+  <si>
+    <t>bejko</t>
+  </si>
+  <si>
+    <t>migena</t>
+  </si>
+  <si>
+    <t>54211323</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>strasbuorg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -169,8 +191,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,52 +472,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A8" sqref="A8:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1">
@@ -504,137 +526,167 @@
       <c r="E2" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1">
         <v>67000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="H7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>